<commit_message>
refractoring sections 2 and 3
</commit_message>
<xml_diff>
--- a/excels/TLB_reach.xlsx
+++ b/excels/TLB_reach.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jevdjic/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jevdjic/Desktop/spryvm/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93305201-66CC-674F-AB79-EE0E6BCDD4DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79404022-475B-AD40-BA9C-F26B5ED1EACA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11420" yWindow="640" windowWidth="24680" windowHeight="15000" xr2:uid="{0A1E2026-DC99-8E42-8C6A-4C992114451A}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="24680" windowHeight="15000" xr2:uid="{0A1E2026-DC99-8E42-8C6A-4C992114451A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,10 +396,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$6:$O$20</c:f>
+              <c:f>Sheet1!$O$6:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.1796875</c:v>
                 </c:pt>
@@ -443,6 +443,9 @@
                   <c:v>32768.29296875</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>65537.4765625</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>147456.33203125</c:v>
                 </c:pt>
               </c:numCache>
@@ -450,10 +453,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$P$6:$P$20</c:f>
+              <c:f>Sheet1!$P$6:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.10692663589699999</c:v>
                 </c:pt>
@@ -497,6 +500,9 @@
                   <c:v>31.2838882179</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>32.9915434901</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>43.366664771400004</c:v>
                 </c:pt>
               </c:numCache>
@@ -549,10 +555,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$R$6:$R$20</c:f>
+              <c:f>Sheet1!$R$6:$R$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.125</c:v>
                 </c:pt>
@@ -597,16 +603,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>32768.09375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>130693.62109375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$S$6:$S$20</c:f>
+              <c:f>Sheet1!$S$6:$S$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.3895918548600001E-7</c:v>
                 </c:pt>
@@ -651,6 +660,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.8140494773500002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.3718414125800003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,10 +714,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$6:$U$20</c:f>
+              <c:f>Sheet1!$U$6:$U$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.125</c:v>
                 </c:pt>
@@ -750,16 +762,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>32768.09375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>130026.80078125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$6:$V$20</c:f>
+              <c:f>Sheet1!$V$6:$V$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.12077739831500001</c:v>
                 </c:pt>
@@ -804,6 +819,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>18.673148983000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.986601961200002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,6 +976,7 @@
         <c:axId val="859001888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="45"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1727,13 +1746,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>730250</xdr:colOff>
+      <xdr:colOff>730249</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>751267</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590282</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>125211</xdr:rowOff>
     </xdr:to>
@@ -2062,14 +2081,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E6D6A2-E68C-994E-AE55-F77806D8904E}">
   <dimension ref="A2:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
@@ -2132,11 +2152,11 @@
         <v>736</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D18" si="0">B5-C5</f>
+        <f t="shared" ref="D5:D19" si="0">B5-C5</f>
         <v>164</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E18" si="1">D5/1024</f>
+        <f t="shared" ref="E5:E19" si="1">D5/1024</f>
         <v>0.16015625</v>
       </c>
       <c r="F5" s="7">
@@ -2754,6 +2774,26 @@
       </c>
     </row>
     <row r="19" spans="1:22">
+      <c r="A19" s="3">
+        <v>33554432</v>
+      </c>
+      <c r="B19" s="3">
+        <v>67110752</v>
+      </c>
+      <c r="C19">
+        <v>736</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>67110016</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>65537.125</v>
+      </c>
+      <c r="F19" s="3">
+        <v>5.5313407482899999</v>
+      </c>
       <c r="L19">
         <v>5626.31640625</v>
       </c>
@@ -2780,6 +2820,26 @@
       </c>
     </row>
     <row r="20" spans="1:22">
+      <c r="A20" s="3">
+        <v>67108864</v>
+      </c>
+      <c r="B20" s="3">
+        <v>133831004</v>
+      </c>
+      <c r="C20">
+        <v>736</v>
+      </c>
+      <c r="D20">
+        <f>B20-C20</f>
+        <v>133830268</v>
+      </c>
+      <c r="E20">
+        <f>D20/1024</f>
+        <v>130693.62109375</v>
+      </c>
+      <c r="F20" s="3">
+        <v>6.3718414125800003</v>
+      </c>
       <c r="L20">
         <v>22594.32421875</v>
       </c>
@@ -2787,10 +2847,10 @@
         <v>16.142295809099998</v>
       </c>
       <c r="O20">
-        <v>147456.33203125</v>
+        <v>65537.4765625</v>
       </c>
       <c r="P20">
-        <v>43.366664771400004</v>
+        <v>32.9915434901</v>
       </c>
       <c r="R20">
         <v>32768.09375</v>
@@ -2812,6 +2872,24 @@
       <c r="M21">
         <v>18.667358348600001</v>
       </c>
+      <c r="O21">
+        <v>147456.33203125</v>
+      </c>
+      <c r="P21">
+        <v>43.366664771400004</v>
+      </c>
+      <c r="R21">
+        <v>130693.62109375</v>
+      </c>
+      <c r="S21">
+        <v>6.3718414125800003</v>
+      </c>
+      <c r="U21">
+        <v>130026.80078125</v>
+      </c>
+      <c r="V21">
+        <v>23.986601961200002</v>
+      </c>
     </row>
     <row r="22" spans="1:22">
       <c r="B22" s="1"/>
@@ -2875,11 +2953,11 @@
         <v>736</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D39" si="2">B26-C26</f>
+        <f t="shared" ref="D26:D40" si="2">B26-C26</f>
         <v>160</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26:E39" si="3">D26/1024</f>
+        <f t="shared" ref="E26:E40" si="3">D26/1024</f>
         <v>0.15625</v>
       </c>
       <c r="F26" s="1">
@@ -3191,12 +3269,52 @@
       <c r="Q39" s="4"/>
     </row>
     <row r="40" spans="1:17">
+      <c r="A40" s="3">
+        <v>33554432</v>
+      </c>
+      <c r="B40" s="3">
+        <v>67110788</v>
+      </c>
+      <c r="C40" s="2">
+        <v>736</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>67110052</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>65537.16015625</v>
+      </c>
+      <c r="F40" s="3">
+        <v>22.015159343800001</v>
+      </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="O40" s="4"/>
       <c r="Q40" s="4"/>
     </row>
     <row r="41" spans="1:17">
+      <c r="A41" s="3">
+        <v>67108864</v>
+      </c>
+      <c r="B41" s="3">
+        <v>133148180</v>
+      </c>
+      <c r="C41" s="2">
+        <v>736</v>
+      </c>
+      <c r="D41">
+        <f>B41-C41</f>
+        <v>133147444</v>
+      </c>
+      <c r="E41">
+        <f>D41/1024</f>
+        <v>130026.80078125</v>
+      </c>
+      <c r="F41" s="3">
+        <v>23.986601961200002</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="O41" s="4"/>
@@ -3573,24 +3691,46 @@
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="1">
-        <v>16777216</v>
+      <c r="A61" s="3">
+        <v>8388608</v>
       </c>
       <c r="B61" s="3">
-        <v>150996020</v>
+        <v>67111112</v>
       </c>
       <c r="C61" s="2">
         <v>736</v>
       </c>
       <c r="D61">
         <f t="shared" si="6"/>
-        <v>150995284</v>
+        <v>67110376</v>
       </c>
       <c r="E61">
         <f t="shared" si="7"/>
+        <v>65537.4765625</v>
+      </c>
+      <c r="F61" s="3">
+        <v>32.9915434901</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="1">
+        <v>16777216</v>
+      </c>
+      <c r="B62" s="3">
+        <v>150996020</v>
+      </c>
+      <c r="C62" s="2">
+        <v>736</v>
+      </c>
+      <c r="D62">
+        <f>B62-C62</f>
+        <v>150995284</v>
+      </c>
+      <c r="E62">
+        <f>D62/1024</f>
         <v>147456.33203125</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F62" s="1">
         <v>43.366664771400004</v>
       </c>
     </row>
@@ -3740,11 +3880,11 @@
         <v>736</v>
       </c>
       <c r="D76">
-        <f t="shared" ref="D76:D87" si="8">B76-C76</f>
+        <f t="shared" ref="D76:D85" si="8">B76-C76</f>
         <v>2040</v>
       </c>
       <c r="E76">
-        <f t="shared" ref="E76:E87" si="9">D76/1024</f>
+        <f t="shared" ref="E76:E85" si="9">D76/1024</f>
         <v>1.9921875</v>
       </c>
       <c r="F76" s="1">

</xml_diff>

<commit_message>
added overview figure and fixed TLB reach figure
</commit_message>
<xml_diff>
--- a/excels/TLB_reach.xlsx
+++ b/excels/TLB_reach.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jevdjic/Desktop/spryvm/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F3B0F-E0BD-8345-B333-45238CB72CCC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E662028-6D8C-8B4B-9470-60B23FFFA1F9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="24680" windowHeight="15000" xr2:uid="{0A1E2026-DC99-8E42-8C6A-4C992114451A}"/>
+    <workbookView xWindow="1280" yWindow="640" windowWidth="45000" windowHeight="21980" xr2:uid="{0A1E2026-DC99-8E42-8C6A-4C992114451A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +119,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -140,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -150,6 +156,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,7 +228,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="star"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -287,7 +294,7 @@
                   <c:v>22594.32421875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44850.33984375</c:v>
+                  <c:v>45043.33984375</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>114709.45703125</c:v>
@@ -347,7 +354,7 @@
                   <c:v>16.142295809099998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.667358348600001</c:v>
+                  <c:v>17.0137067396</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>18.234834260100001</c:v>
@@ -386,7 +393,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -538,7 +545,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -549,7 +556,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -704,7 +711,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -2087,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E6D6A2-E68C-994E-AE55-F77806D8904E}">
   <dimension ref="A2:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2873,10 +2880,10 @@
     </row>
     <row r="21" spans="1:22">
       <c r="L21">
-        <v>44850.33984375</v>
+        <v>45043.33984375</v>
       </c>
       <c r="M21">
-        <v>18.667358348600001</v>
+        <v>17.0137067396</v>
       </c>
       <c r="O21">
         <v>147456.33203125</v>
@@ -4101,26 +4108,26 @@
         <v>16.142295809099998</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" ht="20">
       <c r="A86">
         <v>33554432</v>
       </c>
-      <c r="B86" s="1">
-        <v>45927484</v>
+      <c r="B86" s="9">
+        <v>46125116</v>
       </c>
       <c r="C86" s="2">
         <v>736</v>
       </c>
       <c r="D86">
         <f>B86-C86</f>
-        <v>45926748</v>
+        <v>46124380</v>
       </c>
       <c r="E86">
         <f>D86/1024</f>
-        <v>44850.33984375</v>
-      </c>
-      <c r="F86" s="1">
-        <v>18.667358348600001</v>
+        <v>45043.33984375</v>
+      </c>
+      <c r="F86" s="9">
+        <v>17.0137067396</v>
       </c>
     </row>
     <row r="87" spans="1:6">

</xml_diff>